<commit_message>
Save sheet data through XmlWriter 1/18 - Text file "RemoveExistingStrings" had an explicitely stated outlineLevel="0" despite "0" being the default.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/InlineStrings/outputfile.xlsx
+++ b/ClosedXML.Tests/Resource/Other/InlineStrings/outputfile.xlsx
@@ -541,7 +541,7 @@
   <x:sheetFormatPr defaultRowHeight="14.3"/>
   <x:sheetData>
     <x:row r="1" spans="1:2" hidden="1"/>
-    <x:row r="2" spans="1:2" outlineLevel="0">
+    <x:row r="2" spans="1:2">
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -549,7 +549,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2" outlineLevel="0">
+    <x:row r="3" spans="1:2">
       <x:c r="A3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -557,7 +557,7 @@
         <x:v>64</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2" outlineLevel="0">
+    <x:row r="4" spans="1:2">
       <x:c r="A4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -565,7 +565,7 @@
         <x:v>2494</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:2" outlineLevel="0">
+    <x:row r="5" spans="1:2">
       <x:c r="A5" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -573,7 +573,7 @@
         <x:v>10041</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:2" outlineLevel="0">
+    <x:row r="6" spans="1:2">
       <x:c r="A6" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
@@ -581,7 +581,7 @@
         <x:v>61631</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:2" outlineLevel="0">
+    <x:row r="7" spans="1:2">
       <x:c r="A7" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -589,7 +589,7 @@
         <x:v>293</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:2" outlineLevel="0">
+    <x:row r="8" spans="1:2">
       <x:c r="A8" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -597,7 +597,7 @@
         <x:v>40120</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:2" outlineLevel="0">
+    <x:row r="9" spans="1:2">
       <x:c r="A9" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
@@ -605,7 +605,7 @@
         <x:v>82</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:2" outlineLevel="0">
+    <x:row r="10" spans="1:2">
       <x:c r="A10" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -613,7 +613,7 @@
         <x:v>96621</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:2" outlineLevel="0">
+    <x:row r="11" spans="1:2">
       <x:c r="A11" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -621,7 +621,7 @@
         <x:v>613844</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:2" outlineLevel="0">
+    <x:row r="12" spans="1:2">
       <x:c r="A12" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -629,7 +629,7 @@
         <x:v>79917</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:2" outlineLevel="0">
+    <x:row r="13" spans="1:2">
       <x:c r="A13" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -637,7 +637,7 @@
         <x:v>59172</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:2" outlineLevel="0">
+    <x:row r="14" spans="1:2">
       <x:c r="A14" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
@@ -645,7 +645,7 @@
         <x:v>8464</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:2" outlineLevel="0">
+    <x:row r="15" spans="1:2">
       <x:c r="A15" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -653,7 +653,7 @@
         <x:v>13917</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:2" outlineLevel="0">
+    <x:row r="16" spans="1:2">
       <x:c r="A16" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -661,7 +661,7 @@
         <x:v>366105</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:2" outlineLevel="0">
+    <x:row r="17" spans="1:2">
       <x:c r="A17" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
@@ -669,7 +669,7 @@
         <x:v>130540</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:2" outlineLevel="0">
+    <x:row r="18" spans="1:2">
       <x:c r="A18" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
@@ -677,7 +677,7 @@
         <x:v>2465</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:2" outlineLevel="0">
+    <x:row r="19" spans="1:2">
       <x:c r="A19" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
@@ -685,7 +685,7 @@
         <x:v>21737</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:2" outlineLevel="0">
+    <x:row r="20" spans="1:2">
       <x:c r="A20" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -693,7 +693,7 @@
         <x:v>47578</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:2" outlineLevel="0">
+    <x:row r="21" spans="1:2">
       <x:c r="A21" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -701,7 +701,7 @@
         <x:v>25007</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:2" outlineLevel="0">
+    <x:row r="22" spans="1:2">
       <x:c r="A22" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -709,7 +709,7 @@
         <x:v>186534</x:v>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:2" outlineLevel="0">
+    <x:row r="23" spans="1:2">
       <x:c r="A23" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
@@ -717,7 +717,7 @@
         <x:v>88108</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:2" outlineLevel="0">
+    <x:row r="24" spans="1:2">
       <x:c r="A24" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
@@ -725,7 +725,7 @@
         <x:v>41361</x:v>
       </x:c>
     </x:row>
-    <x:row r="25" spans="1:2" outlineLevel="0">
+    <x:row r="25" spans="1:2">
       <x:c r="A25" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -733,7 +733,7 @@
         <x:v>59488</x:v>
       </x:c>
     </x:row>
-    <x:row r="26" spans="1:2" outlineLevel="0">
+    <x:row r="26" spans="1:2">
       <x:c r="A26" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
@@ -741,7 +741,7 @@
         <x:v>59583</x:v>
       </x:c>
     </x:row>
-    <x:row r="27" spans="1:2" outlineLevel="0">
+    <x:row r="27" spans="1:2">
       <x:c r="A27" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
@@ -749,7 +749,7 @@
         <x:v>120485</x:v>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:2" outlineLevel="0">
+    <x:row r="28" spans="1:2">
       <x:c r="A28" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
@@ -757,7 +757,7 @@
         <x:v>92578</x:v>
       </x:c>
     </x:row>
-    <x:row r="29" spans="1:2" outlineLevel="0">
+    <x:row r="29" spans="1:2">
       <x:c r="A29" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -765,7 +765,7 @@
         <x:v>19889</x:v>
       </x:c>
     </x:row>
-    <x:row r="30" spans="1:2" outlineLevel="0">
+    <x:row r="30" spans="1:2">
       <x:c r="A30" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -773,7 +773,7 @@
         <x:v>149924</x:v>
       </x:c>
     </x:row>
-    <x:row r="31" spans="1:2" outlineLevel="0">
+    <x:row r="31" spans="1:2">
       <x:c r="A31" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
@@ -781,7 +781,7 @@
         <x:v>94877</x:v>
       </x:c>
     </x:row>
-    <x:row r="32" spans="1:2" outlineLevel="0">
+    <x:row r="32" spans="1:2">
       <x:c r="A32" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
@@ -789,7 +789,7 @@
         <x:v>83686</x:v>
       </x:c>
     </x:row>
-    <x:row r="33" spans="1:2" outlineLevel="0">
+    <x:row r="33" spans="1:2">
       <x:c r="A33" s="0" t="s">
         <x:v>32</x:v>
       </x:c>
@@ -797,7 +797,7 @@
         <x:v>406</x:v>
       </x:c>
     </x:row>
-    <x:row r="34" spans="1:2" outlineLevel="0">
+    <x:row r="34" spans="1:2">
       <x:c r="A34" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
@@ -805,7 +805,7 @@
         <x:v>35746</x:v>
       </x:c>
     </x:row>
-    <x:row r="35" spans="1:2" outlineLevel="0">
+    <x:row r="35" spans="1:2">
       <x:c r="A35" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
@@ -813,7 +813,7 @@
         <x:v>15699</x:v>
       </x:c>
     </x:row>
-    <x:row r="36" spans="1:2" outlineLevel="0">
+    <x:row r="36" spans="1:2">
       <x:c r="A36" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -821,7 +821,7 @@
         <x:v>142274</x:v>
       </x:c>
     </x:row>
-    <x:row r="37" spans="1:2" outlineLevel="0">
+    <x:row r="37" spans="1:2">
       <x:c r="A37" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
@@ -829,7 +829,7 @@
         <x:v>12755</x:v>
       </x:c>
     </x:row>
-    <x:row r="38" spans="1:2" outlineLevel="0">
+    <x:row r="38" spans="1:2">
       <x:c r="A38" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
@@ -837,7 +837,7 @@
         <x:v>29806</x:v>
       </x:c>
     </x:row>
-    <x:row r="39" spans="1:2" outlineLevel="0">
+    <x:row r="39" spans="1:2">
       <x:c r="A39" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
@@ -845,7 +845,7 @@
         <x:v>22771</x:v>
       </x:c>
     </x:row>
-    <x:row r="40" spans="1:2" outlineLevel="0">
+    <x:row r="40" spans="1:2">
       <x:c r="A40" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
@@ -853,7 +853,7 @@
         <x:v>157926</x:v>
       </x:c>
     </x:row>
-    <x:row r="41" spans="1:2" outlineLevel="0">
+    <x:row r="41" spans="1:2">
       <x:c r="A41" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
@@ -861,7 +861,7 @@
         <x:v>25904</x:v>
       </x:c>
     </x:row>
-    <x:row r="42" spans="1:2" outlineLevel="0">
+    <x:row r="42" spans="1:2">
       <x:c r="A42" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
@@ -869,7 +869,7 @@
         <x:v>44534</x:v>
       </x:c>
     </x:row>
-    <x:row r="43" spans="1:2" outlineLevel="0">
+    <x:row r="43" spans="1:2">
       <x:c r="A43" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
@@ -877,7 +877,7 @@
         <x:v>342298</x:v>
       </x:c>
     </x:row>
-    <x:row r="44" spans="1:2" outlineLevel="0">
+    <x:row r="44" spans="1:2">
       <x:c r="A44" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
@@ -885,7 +885,7 @@
         <x:v>185713</x:v>
       </x:c>
     </x:row>
-    <x:row r="45" spans="1:2" outlineLevel="0">
+    <x:row r="45" spans="1:2">
       <x:c r="A45" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
@@ -893,7 +893,7 @@
         <x:v>48861</x:v>
       </x:c>
     </x:row>
-    <x:row r="46" spans="1:2" outlineLevel="0">
+    <x:row r="46" spans="1:2">
       <x:c r="A46" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
@@ -901,7 +901,7 @@
         <x:v>65474</x:v>
       </x:c>
     </x:row>
-    <x:row r="47" spans="1:2" outlineLevel="0">
+    <x:row r="47" spans="1:2">
       <x:c r="A47" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
@@ -909,7 +909,7 @@
         <x:v>203386</x:v>
       </x:c>
     </x:row>
-    <x:row r="48" spans="1:2" outlineLevel="0">
+    <x:row r="48" spans="1:2">
       <x:c r="A48" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
@@ -917,7 +917,7 @@
         <x:v>52344</x:v>
       </x:c>
     </x:row>
-    <x:row r="49" spans="1:2" outlineLevel="0">
+    <x:row r="49" spans="1:2">
       <x:c r="A49" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
@@ -925,7 +925,7 @@
         <x:v>19816</x:v>
       </x:c>
     </x:row>
-    <x:row r="50" spans="1:2" outlineLevel="0">
+    <x:row r="50" spans="1:2">
       <x:c r="A50" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
@@ -933,7 +933,7 @@
         <x:v>65340</x:v>
       </x:c>
     </x:row>
-    <x:row r="51" spans="1:2" outlineLevel="0">
+    <x:row r="51" spans="1:2">
       <x:c r="A51" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
@@ -941,7 +941,7 @@
         <x:v>13427</x:v>
       </x:c>
     </x:row>
-    <x:row r="52" spans="1:2" outlineLevel="0">
+    <x:row r="52" spans="1:2">
       <x:c r="A52" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
@@ -949,7 +949,7 @@
         <x:v>91541</x:v>
       </x:c>
     </x:row>
-    <x:row r="53" spans="1:2" outlineLevel="0">
+    <x:row r="53" spans="1:2">
       <x:c r="A53" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
@@ -957,7 +957,7 @@
         <x:v>394702</x:v>
       </x:c>
     </x:row>
-    <x:row r="54" spans="1:2" outlineLevel="0">
+    <x:row r="54" spans="1:2">
       <x:c r="A54" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
@@ -965,7 +965,7 @@
         <x:v>42780</x:v>
       </x:c>
     </x:row>
-    <x:row r="55" spans="1:2" outlineLevel="0">
+    <x:row r="55" spans="1:2">
       <x:c r="A55" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
@@ -973,7 +973,7 @@
         <x:v>126069</x:v>
       </x:c>
     </x:row>
-    <x:row r="56" spans="1:2" outlineLevel="0">
+    <x:row r="56" spans="1:2">
       <x:c r="A56" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
@@ -981,7 +981,7 @@
         <x:v>1150</x:v>
       </x:c>
     </x:row>
-    <x:row r="57" spans="1:2" outlineLevel="0">
+    <x:row r="57" spans="1:2">
       <x:c r="A57" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -989,7 +989,7 @@
         <x:v>10051</x:v>
       </x:c>
     </x:row>
-    <x:row r="58" spans="1:2" outlineLevel="0">
+    <x:row r="58" spans="1:2">
       <x:c r="A58" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
@@ -997,7 +997,7 @@
         <x:v>115953</x:v>
       </x:c>
     </x:row>
-    <x:row r="59" spans="1:2" outlineLevel="0">
+    <x:row r="59" spans="1:2">
       <x:c r="A59" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
@@ -1005,7 +1005,7 @@
         <x:v>85362</x:v>
       </x:c>
     </x:row>
-    <x:row r="60" spans="1:2" outlineLevel="0">
+    <x:row r="60" spans="1:2">
       <x:c r="A60" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
@@ -1013,7 +1013,7 @@
         <x:v>25646</x:v>
       </x:c>
     </x:row>
-    <x:row r="61" spans="1:2" outlineLevel="0">
+    <x:row r="61" spans="1:2">
       <x:c r="A61" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
@@ -1021,7 +1021,7 @@
         <x:v>8352</x:v>
       </x:c>
     </x:row>
-    <x:row r="63" spans="1:2" outlineLevel="0">
+    <x:row r="63" spans="1:2">
       <x:c r="A63" s="0" t="s">
         <x:v>61</x:v>
       </x:c>

</xml_diff>